<commit_message>
code to generate graphs
code to generate graphs for the metrics.
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CDADM1.0\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0B9F14-2789-4285-B565-B4B57D260702}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FC34CE-1175-4EEE-8496-7EB4879C3B89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{473CD6AC-FCF0-45FA-A0D8-FB91AB211D7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{473CD6AC-FCF0-45FA-A0D8-FB91AB211D7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Across Domain" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -179,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Metric</t>
   </si>
@@ -213,12 +214,36 @@
   <si>
     <t>Consistent across domains</t>
   </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Baseline Accuracy</t>
+  </si>
+  <si>
+    <t>CDADM Accuracy</t>
+  </si>
+  <si>
+    <t>Baseline F1-Score</t>
+  </si>
+  <si>
+    <t>CDADM F1-Score</t>
+  </si>
+  <si>
+    <t>Computer Vision</t>
+  </si>
+  <si>
+    <t>Natural Language Processing (NLP)</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +276,40 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,11 +353,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -307,6 +363,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,7 +951,1364 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Metrics comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> across Domains</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Across Domain'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Across Domain'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Computer Vision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Natural Language Processing (NLP)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cybersecurity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Across Domain'!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FAF8-446A-8130-0EA1614544D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Across Domain'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDADM Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Across Domain'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Computer Vision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Natural Language Processing (NLP)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cybersecurity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Across Domain'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FAF8-446A-8130-0EA1614544D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1847625568"/>
+        <c:axId val="1579375392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1847625568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Domain</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1579375392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1579375392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1847625568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>F1 score comparison across domains</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Across Domain'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline F1-Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Across Domain'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Computer Vision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Natural Language Processing (NLP)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cybersecurity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Across Domain'!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74B8-4FE6-9378-9ACCBF8E0A7E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Across Domain'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDADM F1-Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Across Domain'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Computer Vision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Natural Language Processing (NLP)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cybersecurity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Across Domain'!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-74B8-4FE6-9378-9ACCBF8E0A7E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1857528272"/>
+        <c:axId val="1849088032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1857528272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Domain</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1849088032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1849088032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>F1 score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1857528272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1418,6 +2851,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1451,6 +3890,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1089660</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AA5E195-9D4E-471A-BE89-37956BB58A63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>899160</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{150D92E0-A939-457F-8A34-92DF8381B85E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1756,27 +4272,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B07ED6-319B-447D-BFFD-F6767E81C76E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1784,10 +4300,10 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.85</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.9</v>
       </c>
     </row>
@@ -1795,10 +4311,10 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.85</v>
       </c>
     </row>
@@ -1806,10 +4322,10 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.65</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.92</v>
       </c>
     </row>
@@ -1817,10 +4333,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.15</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.08</v>
       </c>
     </row>
@@ -1828,22 +4344,88 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.05</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -1852,4 +4434,140 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B958FE-EA95-4318-8A44-E61F42075856}">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.82</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.91</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.78</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="C32" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0.83</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0.87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>